<commit_message>
add slides about Parser
</commit_message>
<xml_diff>
--- a/core/src/main/resources/example.xlsx
+++ b/core/src/main/resources/example.xlsx
@@ -4,15 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="25940" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="GasLossFactor">Sheet1!$B$4</definedName>
+    <definedName name="ExplorationFee">Sheet1!$B$13</definedName>
+    <definedName name="GasLossFactor">Sheet1!$B$5</definedName>
     <definedName name="GasProd">Sheet1!$B$8:$J$8</definedName>
     <definedName name="OilProd">Sheet1!$B$7:$J$7</definedName>
+    <definedName name="PostExplorationFee">Sheet1!$B$14</definedName>
+    <definedName name="PrimaryProduct">Sheet1!$B$4</definedName>
+    <definedName name="Years">Sheet1!$B$2:$J$2</definedName>
   </definedNames>
   <calcPr calcId="140000" calcMode="autoNoTable" concurrentCalc="0"/>
   <extLst>
@@ -24,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Production</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>oil</t>
   </si>
@@ -39,13 +40,28 @@
   </si>
   <si>
     <t>gas loss factor</t>
+  </si>
+  <si>
+    <t>primary product</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>Fee</t>
+  </si>
+  <si>
+    <t>exploration</t>
+  </si>
+  <si>
+    <t>post exploration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -53,41 +69,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9948118533890809E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -102,12 +90,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J8"/>
+  <dimension ref="A2:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -452,7 +439,7 @@
   <sheetData>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>2017</v>
@@ -486,27 +473,21 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="20">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7">
         <v>10.119999999999999</v>
@@ -538,7 +519,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -566,6 +547,27 @@
       </c>
       <c r="J8">
         <v>6.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>5.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove gas loss factor
</commit_message>
<xml_diff>
--- a/core/src/main/resources/example.xlsx
+++ b/core/src/main/resources/example.xlsx
@@ -10,11 +10,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExplorationFee">Sheet1!$B$13</definedName>
-    <definedName name="GasLossFactor">Sheet1!$B$5</definedName>
-    <definedName name="GasProd">Sheet1!$B$8:$J$8</definedName>
-    <definedName name="OilProd">Sheet1!$B$7:$J$7</definedName>
-    <definedName name="PostExplorationFee">Sheet1!$B$14</definedName>
+    <definedName name="ExplorationFee">Sheet1!$B$12</definedName>
+    <definedName name="GasLossFactor">Sheet1!#REF!</definedName>
+    <definedName name="GasProd">Sheet1!$B$7:$J$7</definedName>
+    <definedName name="OilProd">Sheet1!$B$6:$J$6</definedName>
+    <definedName name="PostExplorationFee">Sheet1!$B$13</definedName>
     <definedName name="PrimaryProduct">Sheet1!$B$4</definedName>
     <definedName name="Years">Sheet1!$B$2:$J$2</definedName>
   </definedNames>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>oil</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Year</t>
-  </si>
-  <si>
-    <t>gas loss factor</t>
   </si>
   <si>
     <t>primary product</t>
@@ -426,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J14"/>
+  <dimension ref="A2:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -471,102 +468,94 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>0.02</v>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>10.119999999999999</v>
+      </c>
+      <c r="C6">
+        <v>12.34</v>
+      </c>
+      <c r="D6">
+        <v>8.83</v>
+      </c>
+      <c r="E6">
+        <v>6.23</v>
+      </c>
+      <c r="F6">
+        <v>9.18</v>
+      </c>
+      <c r="G6">
+        <v>12.36</v>
+      </c>
+      <c r="H6">
+        <v>16.28</v>
+      </c>
+      <c r="I6">
+        <v>18.25</v>
+      </c>
+      <c r="J6">
+        <v>20.010000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
         <v>0</v>
       </c>
-      <c r="B7">
-        <v>10.119999999999999</v>
-      </c>
       <c r="C7">
-        <v>12.34</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>8.83</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>6.23</v>
+        <v>3.2</v>
       </c>
       <c r="F7">
-        <v>9.18</v>
+        <v>6.5</v>
       </c>
       <c r="G7">
-        <v>12.36</v>
+        <v>6.38</v>
       </c>
       <c r="H7">
-        <v>16.28</v>
+        <v>5.72</v>
       </c>
       <c r="I7">
-        <v>18.25</v>
+        <v>4.54</v>
       </c>
       <c r="J7">
-        <v>20.010000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>3.2</v>
-      </c>
-      <c r="F8">
-        <v>6.5</v>
-      </c>
-      <c r="G8">
-        <v>6.38</v>
-      </c>
-      <c r="H8">
-        <v>5.72</v>
-      </c>
-      <c r="I8">
-        <v>4.54</v>
-      </c>
-      <c r="J8">
         <v>6.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>6</v>
       </c>
+      <c r="B12">
+        <v>1.4</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14">
         <v>5.8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add sequential dependency slides
</commit_message>
<xml_diff>
--- a/core/src/main/resources/example.xlsx
+++ b/core/src/main/resources/example.xlsx
@@ -10,11 +10,13 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExplorationFee">Sheet1!$B$12</definedName>
-    <definedName name="GasLossFactor">Sheet1!#REF!</definedName>
+    <definedName name="Cost">Sheet1!$B$15</definedName>
+    <definedName name="ExplorationFee">Sheet1!$B$11</definedName>
     <definedName name="GasProd">Sheet1!$B$7:$J$7</definedName>
+    <definedName name="HardcodedCost">Sheet1!$B$16:$J$16</definedName>
     <definedName name="OilProd">Sheet1!$B$6:$J$6</definedName>
-    <definedName name="PostExplorationFee">Sheet1!$B$13</definedName>
+    <definedName name="ParametrizedCost">Sheet1!$B$17</definedName>
+    <definedName name="PostExplorationFee">Sheet1!$B$12</definedName>
     <definedName name="PrimaryProduct">Sheet1!$B$4</definedName>
     <definedName name="Years">Sheet1!$B$2:$J$2</definedName>
   </definedNames>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>oil</t>
   </si>
@@ -52,16 +54,41 @@
   </si>
   <si>
     <t>post exploration</t>
+  </si>
+  <si>
+    <t>harcoded</t>
+  </si>
+  <si>
+    <t>parametrized</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,8 +111,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -93,7 +126,13 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -423,15 +462,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J13"/>
+  <dimension ref="A2:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10">
@@ -538,29 +577,78 @@
         <v>6.99</v>
       </c>
     </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>1.4</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B12">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13">
         <v>5.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>12.3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>